<commit_message>
fix deletion and double-string conversion
</commit_message>
<xml_diff>
--- a/templates/people-and-taxes.xlsx
+++ b/templates/people-and-taxes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Тарифы</t>
   </si>
@@ -65,15 +65,6 @@
   </si>
   <si>
     <t>Услуги</t>
-  </si>
-  <si>
-    <t>Амиджаев С.И.</t>
-  </si>
-  <si>
-    <t>201, 202</t>
-  </si>
-  <si>
-    <t>30,5</t>
   </si>
   <si>
     <t>Кол-во прожи-вающих</t>
@@ -124,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -240,54 +231,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q10"/>
+  <dimension ref="A2:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -622,141 +736,149 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" s="6" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="6" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10" t="s">
+    <row r="9" spans="1:17" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="10" t="s">
+      <c r="M9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="11"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="8"/>
     </row>
-    <row r="10" spans="1:17" s="13" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>44</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="13">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="13">
-        <v>5</v>
-      </c>
-      <c r="G10" s="15">
-        <v>158.6</v>
-      </c>
-      <c r="H10" s="15">
-        <v>1462.78</v>
-      </c>
-      <c r="I10" s="15">
-        <v>252</v>
-      </c>
-      <c r="J10" s="15">
-        <v>2466</v>
-      </c>
-      <c r="K10" s="15">
-        <v>208.3</v>
-      </c>
-      <c r="L10" s="15">
-        <v>523.38</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15">
-        <v>2851.66</v>
-      </c>
-      <c r="O10" s="15">
-        <v>2910</v>
-      </c>
-      <c r="P10" s="15">
-        <v>2909.22</v>
-      </c>
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:N8"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>